<commit_message>
Updates to the script in coordination with a fix with soil textures in the RHEM web service
</commit_message>
<xml_diff>
--- a/RHEM_template.xlsx
+++ b/RHEM_template.xlsx
@@ -1,30 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gerardo/my/Projects/RHEM/RHEM_batch_app/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BFEC919-CFFF-9D47-824B-B43BFBF454E3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="51200" windowHeight="28280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Inputs" sheetId="1" r:id="rId1"/>
-    <sheet name="Lookup Tables" sheetId="2" r:id="rId2"/>
+    <sheet name="Inputs" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Lookup Tables" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="Uniform">Inputs!$H$2</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="49">
   <si>
     <t>Scenario Name</t>
   </si>
@@ -89,7 +82,7 @@
     <t>Avg SY (ton/ha/year)</t>
   </si>
   <si>
-    <t>NOTE:  Please use the  "Lookup Tables" tab to get the possible values for Units, Soil Texture, and Slope Shape.  To find out climate station IDs, please visit the RHEM Web Tool website (https://apps.tucson.ars.ag.gov/rhem</t>
+    <t>NOTE:  Please use the  "Lookup Tables" tab to get the possible values for Units, Soil Texture, and Slope Shape.  To find the climate station IDs, visit the Climate Station section of the RHEM Web Tool: https://apps.tucson.ars.ag.gov/rhem</t>
   </si>
   <si>
     <t>Scenario_0</t>
@@ -107,7 +100,7 @@
     <t>Uniform</t>
   </si>
   <si>
-    <t xml:space="preserve">        229.18866</t>
+    <t xml:space="preserve">   261.94</t>
   </si>
   <si>
     <t xml:space="preserve">          18.73193</t>
@@ -176,61 +169,70 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="6">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="14"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="14"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="18"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="18"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="14"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="14"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="14"/>
-      <color rgb="FF222222"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color rgb="FF222222"/>
+      <sz val="14"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="18"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
+        <fgColor theme="9" tint="0.5999938962981048"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
+        <fgColor theme="4" tint="0.7999816888943144"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -272,57 +274,48 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="14">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="1" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="1" fillId="3" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="4" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="1" fillId="3" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="1" fillId="3" fontId="1" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="5" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -622,40 +615,44 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:AA7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V16" sqref="V16"/>
+      <selection activeCell="T9" sqref="T9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="18.1640625" style="12" customWidth="1"/>
-    <col min="2" max="2" width="22" style="12" customWidth="1"/>
-    <col min="3" max="3" width="6.1640625" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" style="12" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" style="13" customWidth="1"/>
-    <col min="6" max="6" width="14.83203125" style="12" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.5" style="12" customWidth="1"/>
-    <col min="9" max="9" width="11.5" style="12" customWidth="1"/>
-    <col min="10" max="10" width="11.83203125" style="12" customWidth="1"/>
-    <col min="11" max="11" width="15.83203125" style="12" customWidth="1"/>
-    <col min="12" max="12" width="8" style="12" customWidth="1"/>
-    <col min="13" max="13" width="7.83203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.33203125" style="12" customWidth="1"/>
-    <col min="15" max="15" width="7.1640625" style="12" customWidth="1"/>
-    <col min="16" max="16" width="8" style="12" customWidth="1"/>
-    <col min="17" max="17" width="11.33203125" style="12" customWidth="1"/>
-    <col min="19" max="19" width="21" style="12" customWidth="1"/>
-    <col min="20" max="20" width="16.83203125" style="12" customWidth="1"/>
-    <col min="21" max="21" width="18.33203125" style="12" customWidth="1"/>
-    <col min="22" max="22" width="16.6640625" style="12" customWidth="1"/>
-    <col min="25" max="25" width="108" style="12" customWidth="1"/>
+    <col customWidth="1" max="1" min="1" style="12" width="18.1640625"/>
+    <col customWidth="1" max="2" min="2" style="12" width="22"/>
+    <col bestFit="1" customWidth="1" max="3" min="3" style="12" width="6.1640625"/>
+    <col customWidth="1" max="4" min="4" style="12" width="10.83203125"/>
+    <col customWidth="1" max="5" min="5" style="13" width="12.6640625"/>
+    <col customWidth="1" max="6" min="6" style="12" width="14.83203125"/>
+    <col bestFit="1" customWidth="1" max="7" min="7" style="12" width="13.33203125"/>
+    <col customWidth="1" max="8" min="8" style="12" width="20.5"/>
+    <col customWidth="1" max="9" min="9" style="12" width="11.5"/>
+    <col customWidth="1" max="10" min="10" style="12" width="11.83203125"/>
+    <col customWidth="1" max="11" min="11" style="12" width="15.83203125"/>
+    <col customWidth="1" max="12" min="12" style="12" width="8"/>
+    <col bestFit="1" customWidth="1" max="13" min="13" style="12" width="7.83203125"/>
+    <col customWidth="1" max="14" min="14" style="12" width="7.33203125"/>
+    <col customWidth="1" max="15" min="15" style="12" width="7.1640625"/>
+    <col customWidth="1" max="16" min="16" style="12" width="8"/>
+    <col customWidth="1" max="17" min="17" style="12" width="11.33203125"/>
+    <col customWidth="1" max="19" min="19" style="12" width="21"/>
+    <col customWidth="1" max="20" min="20" style="12" width="16.83203125"/>
+    <col customWidth="1" max="21" min="21" style="12" width="18.33203125"/>
+    <col customWidth="1" max="22" min="22" style="12" width="16.6640625"/>
+    <col customWidth="1" max="25" min="25" style="12" width="108"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="108" customHeight="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="108" r="1" s="12" spans="1:27">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -719,19 +716,19 @@
       <c r="V1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
+      <c r="W1" s="1" t="n"/>
+      <c r="X1" s="1" t="n"/>
       <c r="Y1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="Z1" s="1"/>
-      <c r="AA1" s="1"/>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="Z1" s="1" t="n"/>
+      <c r="AA1" s="1" t="n"/>
+    </row>
+    <row r="2" spans="1:27">
       <c r="A2" t="s">
         <v>22</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="n">
         <v>1</v>
       </c>
       <c r="D2" t="s">
@@ -743,37 +740,37 @@
       <c r="F2" t="s">
         <v>25</v>
       </c>
-      <c r="G2">
+      <c r="G2" t="n">
         <v>50</v>
       </c>
       <c r="H2" t="s">
         <v>26</v>
       </c>
-      <c r="I2">
+      <c r="I2" t="n">
         <v>4</v>
       </c>
-      <c r="J2">
+      <c r="J2" t="n">
         <v>1.4</v>
       </c>
-      <c r="K2">
+      <c r="K2" t="n">
         <v>1.7</v>
       </c>
-      <c r="L2">
+      <c r="L2" t="n">
         <v>3.9</v>
       </c>
-      <c r="M2">
+      <c r="M2" t="n">
         <v>0</v>
       </c>
-      <c r="N2">
+      <c r="N2" t="n">
         <v>0</v>
       </c>
-      <c r="O2">
+      <c r="O2" t="n">
         <v>5</v>
       </c>
-      <c r="P2">
+      <c r="P2" t="n">
         <v>16.7</v>
       </c>
-      <c r="Q2">
+      <c r="Q2" t="n">
         <v>0</v>
       </c>
       <c r="S2" t="s">
@@ -789,97 +786,37 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="S3"/>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="S4"/>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A5"/>
-      <c r="C5"/>
-      <c r="D5"/>
-      <c r="F5"/>
-      <c r="G5"/>
-      <c r="H5"/>
-      <c r="I5"/>
-      <c r="J5"/>
-      <c r="K5"/>
-      <c r="L5"/>
-      <c r="M5"/>
-      <c r="N5"/>
-      <c r="O5"/>
-      <c r="P5"/>
-      <c r="Q5"/>
-      <c r="S5"/>
-      <c r="T5"/>
-      <c r="U5"/>
-      <c r="V5"/>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A6"/>
-      <c r="C6"/>
-      <c r="D6"/>
-      <c r="F6"/>
-      <c r="G6"/>
-      <c r="H6"/>
-      <c r="I6"/>
-      <c r="J6"/>
-      <c r="K6"/>
-      <c r="L6"/>
-      <c r="M6"/>
-      <c r="N6"/>
-      <c r="O6"/>
-      <c r="P6"/>
-      <c r="Q6"/>
-      <c r="S6"/>
-      <c r="T6"/>
-      <c r="U6"/>
-      <c r="V6"/>
-    </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A7"/>
-      <c r="C7"/>
-      <c r="D7"/>
-      <c r="F7"/>
-      <c r="G7"/>
-      <c r="H7"/>
-      <c r="I7"/>
-      <c r="J7"/>
-      <c r="K7"/>
-      <c r="L7"/>
-      <c r="M7"/>
-      <c r="N7"/>
-      <c r="O7"/>
-      <c r="P7"/>
-      <c r="Q7"/>
-      <c r="S7"/>
-      <c r="T7"/>
-      <c r="U7"/>
-      <c r="V7"/>
-    </row>
+    <row r="3" spans="1:27"/>
+    <row r="4" spans="1:27"/>
+    <row r="5" spans="1:27"/>
+    <row r="6" spans="1:27"/>
+    <row r="7" spans="1:27"/>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="5" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="5" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="18" style="12" customWidth="1"/>
-    <col min="2" max="2" width="24.1640625" style="12" customWidth="1"/>
-    <col min="3" max="3" width="24.6640625" style="12" customWidth="1"/>
+    <col customWidth="1" max="1" min="1" style="12" width="18"/>
+    <col customWidth="1" max="2" min="2" style="12" width="24.1640625"/>
+    <col customWidth="1" max="3" min="3" style="12" width="24.6640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+    <row customHeight="1" ht="33" r="1" s="12" spans="1:3">
       <c r="A1" s="8" t="s">
         <v>2</v>
       </c>
@@ -890,7 +827,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="19" r="2" s="12" spans="1:3">
       <c r="A2" s="9" t="s">
         <v>33</v>
       </c>
@@ -901,7 +838,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="19" r="3" s="12" spans="1:3">
       <c r="A3" s="9" t="s">
         <v>35</v>
       </c>
@@ -912,8 +849,8 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
+    <row customHeight="1" ht="19" r="4" s="12" spans="1:3">
+      <c r="A4" s="11" t="n"/>
       <c r="B4" s="10" t="s">
         <v>25</v>
       </c>
@@ -921,8 +858,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
+    <row customHeight="1" ht="19" r="5" s="12" spans="1:3">
+      <c r="A5" s="11" t="n"/>
       <c r="B5" s="10" t="s">
         <v>39</v>
       </c>
@@ -930,71 +867,71 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
+    <row customHeight="1" ht="19" r="6" s="12" spans="1:3">
+      <c r="A6" s="11" t="n"/>
       <c r="B6" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="9"/>
-    </row>
-    <row r="7" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
+      <c r="C6" s="9" t="n"/>
+    </row>
+    <row customHeight="1" ht="19" r="7" s="12" spans="1:3">
+      <c r="A7" s="11" t="n"/>
       <c r="B7" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="9"/>
-    </row>
-    <row r="8" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
+      <c r="C7" s="9" t="n"/>
+    </row>
+    <row customHeight="1" ht="19" r="8" s="12" spans="1:3">
+      <c r="A8" s="11" t="n"/>
       <c r="B8" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="9"/>
-    </row>
-    <row r="9" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="11"/>
+      <c r="C8" s="9" t="n"/>
+    </row>
+    <row customHeight="1" ht="19" r="9" s="12" spans="1:3">
+      <c r="A9" s="11" t="n"/>
       <c r="B9" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C9" s="9"/>
-    </row>
-    <row r="10" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="11"/>
+      <c r="C9" s="9" t="n"/>
+    </row>
+    <row customHeight="1" ht="19" r="10" s="12" spans="1:3">
+      <c r="A10" s="11" t="n"/>
       <c r="B10" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="C10" s="9"/>
-    </row>
-    <row r="11" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
+      <c r="C10" s="9" t="n"/>
+    </row>
+    <row customHeight="1" ht="19" r="11" s="12" spans="1:3">
+      <c r="A11" s="11" t="n"/>
       <c r="B11" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="9"/>
-    </row>
-    <row r="12" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="11"/>
+      <c r="C11" s="9" t="n"/>
+    </row>
+    <row customHeight="1" ht="19" r="12" s="12" spans="1:3">
+      <c r="A12" s="11" t="n"/>
       <c r="B12" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="C12" s="9"/>
-    </row>
-    <row r="13" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="11"/>
+      <c r="C12" s="9" t="n"/>
+    </row>
+    <row customHeight="1" ht="19" r="13" s="12" spans="1:3">
+      <c r="A13" s="11" t="n"/>
       <c r="B13" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="C13" s="9"/>
-    </row>
-    <row r="14" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-    </row>
-    <row r="15" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
+      <c r="C13" s="9" t="n"/>
+    </row>
+    <row customHeight="1" ht="19" r="14" s="12" spans="1:3">
+      <c r="B14" s="7" t="n"/>
+      <c r="C14" s="7" t="n"/>
+    </row>
+    <row customHeight="1" ht="19" r="15" s="12" spans="1:3">
+      <c r="B15" s="7" t="n"/>
+      <c r="C15" s="7" t="n"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix some problems with the validation of slope steepeness and total percent foliar and ground cover.
</commit_message>
<xml_diff>
--- a/RHEM_template.xlsx
+++ b/RHEM_template.xlsx
@@ -1,23 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gerardo/my/Projects/RHEM/RHEM_batch_app/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{975435A8-627A-CB43-BE78-D1159654D3D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="51200" windowHeight="28360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Inputs" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Lookup Tables" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Inputs" sheetId="1" r:id="rId1"/>
+    <sheet name="Lookup Tables" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="Uniform">Inputs!$H$2</definedName>
   </definedNames>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
   <si>
     <t>Scenario Name</t>
   </si>
@@ -85,63 +92,51 @@
     <t>NOTE:  Please use the  "Lookup Tables" tab to get the possible values for Units, Soil Texture, and Slope Shape.  To find the climate station IDs, visit the Climate Station section of the RHEM Web Tool: https://apps.tucson.ars.ag.gov/rhem</t>
   </si>
   <si>
-    <t>Scenario_0</t>
-  </si>
-  <si>
-    <t>NM</t>
-  </si>
-  <si>
-    <t>294426</t>
+    <t>CO</t>
+  </si>
+  <si>
+    <t>053488</t>
+  </si>
+  <si>
+    <t>Silty Clay Loam</t>
+  </si>
+  <si>
+    <t>Concave</t>
+  </si>
+  <si>
+    <t>S-Shaped</t>
+  </si>
+  <si>
+    <t>Soil Types</t>
+  </si>
+  <si>
+    <t>Slope Shape</t>
+  </si>
+  <si>
+    <t>1 (Metric)</t>
+  </si>
+  <si>
+    <t>Sand</t>
+  </si>
+  <si>
+    <t>Uniform</t>
+  </si>
+  <si>
+    <t>2 (English)</t>
+  </si>
+  <si>
+    <t>Loamy Sand</t>
+  </si>
+  <si>
+    <t>Convex</t>
   </si>
   <si>
     <t>Sandy Loam</t>
   </si>
   <si>
-    <t>Uniform</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   261.94</t>
-  </si>
-  <si>
-    <t xml:space="preserve">          18.73193</t>
-  </si>
-  <si>
-    <t xml:space="preserve">          2.47534</t>
-  </si>
-  <si>
-    <t xml:space="preserve">          2.47460</t>
-  </si>
-  <si>
-    <t>Soil Types</t>
-  </si>
-  <si>
-    <t>Slope Shape</t>
-  </si>
-  <si>
-    <t>1 (Metric)</t>
-  </si>
-  <si>
-    <t>Sand</t>
-  </si>
-  <si>
-    <t>2 (English)</t>
-  </si>
-  <si>
-    <t>Loamy Sand</t>
-  </si>
-  <si>
-    <t>Convex</t>
-  </si>
-  <si>
-    <t>Concave</t>
-  </si>
-  <si>
     <t>Loam</t>
   </si>
   <si>
-    <t>S-Shaped</t>
-  </si>
-  <si>
     <t>Silt Loam</t>
   </si>
   <si>
@@ -152,9 +147,6 @@
   </si>
   <si>
     <t>Clay Loam</t>
-  </si>
-  <si>
-    <t>Silty Clay Loam</t>
   </si>
   <si>
     <t>Sandy Clay</t>
@@ -169,70 +161,71 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <b val="1"/>
-      <color theme="1"/>
-      <sz val="14"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="18"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="18"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="14"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="14"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="14"/>
+      <color rgb="FF222222"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color rgb="FF222222"/>
-      <sz val="14"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <name val="Calibri"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <b val="1"/>
-      <color theme="1"/>
-      <sz val="18"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.5999938962981048"/>
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.7999816888943144"/>
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -274,48 +267,61 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+  <cellXfs count="18">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="3" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="4" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="3" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="3" fontId="1" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="5" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -615,44 +621,40 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:AA7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AA3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T9" sqref="T9"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="12" width="18.1640625"/>
-    <col customWidth="1" max="2" min="2" style="12" width="22"/>
-    <col bestFit="1" customWidth="1" max="3" min="3" style="12" width="6.1640625"/>
-    <col customWidth="1" max="4" min="4" style="12" width="10.83203125"/>
-    <col customWidth="1" max="5" min="5" style="13" width="12.6640625"/>
-    <col customWidth="1" max="6" min="6" style="12" width="14.83203125"/>
-    <col bestFit="1" customWidth="1" max="7" min="7" style="12" width="13.33203125"/>
-    <col customWidth="1" max="8" min="8" style="12" width="20.5"/>
-    <col customWidth="1" max="9" min="9" style="12" width="11.5"/>
-    <col customWidth="1" max="10" min="10" style="12" width="11.83203125"/>
-    <col customWidth="1" max="11" min="11" style="12" width="15.83203125"/>
-    <col customWidth="1" max="12" min="12" style="12" width="8"/>
-    <col bestFit="1" customWidth="1" max="13" min="13" style="12" width="7.83203125"/>
-    <col customWidth="1" max="14" min="14" style="12" width="7.33203125"/>
-    <col customWidth="1" max="15" min="15" style="12" width="7.1640625"/>
-    <col customWidth="1" max="16" min="16" style="12" width="8"/>
-    <col customWidth="1" max="17" min="17" style="12" width="11.33203125"/>
-    <col customWidth="1" max="19" min="19" style="12" width="21"/>
-    <col customWidth="1" max="20" min="20" style="12" width="16.83203125"/>
-    <col customWidth="1" max="21" min="21" style="12" width="18.33203125"/>
-    <col customWidth="1" max="22" min="22" style="12" width="16.6640625"/>
-    <col customWidth="1" max="25" min="25" style="12" width="108"/>
+    <col min="1" max="1" width="18.1640625" style="12" customWidth="1"/>
+    <col min="2" max="2" width="22" style="12" customWidth="1"/>
+    <col min="3" max="3" width="6.1640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="12" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" style="13" customWidth="1"/>
+    <col min="6" max="6" width="14.83203125" style="12" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.5" style="12" customWidth="1"/>
+    <col min="9" max="9" width="11.5" style="12" customWidth="1"/>
+    <col min="10" max="10" width="11.83203125" style="12" customWidth="1"/>
+    <col min="11" max="11" width="15.83203125" style="12" customWidth="1"/>
+    <col min="12" max="12" width="8" style="12" customWidth="1"/>
+    <col min="13" max="13" width="7.83203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.33203125" style="12" customWidth="1"/>
+    <col min="15" max="15" width="7.1640625" style="12" customWidth="1"/>
+    <col min="16" max="16" width="8" style="12" customWidth="1"/>
+    <col min="17" max="17" width="11.33203125" style="12" customWidth="1"/>
+    <col min="19" max="19" width="21" style="12" customWidth="1"/>
+    <col min="20" max="20" width="16.83203125" style="12" customWidth="1"/>
+    <col min="21" max="21" width="18.33203125" style="12" customWidth="1"/>
+    <col min="22" max="22" width="16.6640625" style="12" customWidth="1"/>
+    <col min="25" max="25" width="108" style="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="108" r="1" s="12" spans="1:27">
+    <row r="1" spans="1:27" ht="108" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -716,222 +718,223 @@
       <c r="V1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="1" t="n"/>
-      <c r="X1" s="1" t="n"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
       <c r="Y1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="Z1" s="1" t="n"/>
-      <c r="AA1" s="1" t="n"/>
-    </row>
-    <row r="2" spans="1:27">
-      <c r="A2" t="s">
+      <c r="Z1" s="1"/>
+      <c r="AA1" s="1"/>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A2" s="14">
+        <v>1</v>
+      </c>
+      <c r="B2" s="15">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
         <v>22</v>
       </c>
-      <c r="C2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="E2" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="F2" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2">
+        <v>50</v>
+      </c>
+      <c r="H2" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="G2" t="n">
-        <v>50</v>
-      </c>
-      <c r="H2" t="s">
-        <v>26</v>
-      </c>
-      <c r="I2" t="n">
-        <v>4</v>
-      </c>
-      <c r="J2" t="n">
-        <v>1.4</v>
-      </c>
-      <c r="K2" t="n">
-        <v>1.7</v>
-      </c>
-      <c r="L2" t="n">
-        <v>3.9</v>
-      </c>
-      <c r="M2" t="n">
+      <c r="I2" s="15">
+        <v>15.80000019073486</v>
+      </c>
+      <c r="J2" s="15">
         <v>0</v>
       </c>
-      <c r="N2" t="n">
+      <c r="K2" s="15">
         <v>0</v>
       </c>
-      <c r="O2" t="n">
-        <v>5</v>
-      </c>
-      <c r="P2" t="n">
-        <v>16.7</v>
-      </c>
-      <c r="Q2" t="n">
+      <c r="L2" s="15">
+        <v>20</v>
+      </c>
+      <c r="M2" s="15">
         <v>0</v>
       </c>
-      <c r="S2" t="s">
-        <v>27</v>
-      </c>
-      <c r="T2" t="s">
-        <v>28</v>
-      </c>
-      <c r="U2" t="s">
-        <v>29</v>
-      </c>
-      <c r="V2" t="s">
+      <c r="N2" s="15">
+        <v>0</v>
+      </c>
+      <c r="O2" s="15">
+        <v>0</v>
+      </c>
+      <c r="P2" s="15">
         <v>30</v>
       </c>
-    </row>
-    <row r="3" spans="1:27"/>
-    <row r="4" spans="1:27"/>
-    <row r="5" spans="1:27"/>
-    <row r="6" spans="1:27"/>
-    <row r="7" spans="1:27"/>
+      <c r="Q2" s="15">
+        <v>0</v>
+      </c>
+      <c r="S2"/>
+      <c r="T2"/>
+      <c r="U2"/>
+      <c r="V2"/>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A3" s="14"/>
+      <c r="B3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="15"/>
+      <c r="O3" s="15"/>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="15"/>
+    </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="5" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="5" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="12" width="18"/>
-    <col customWidth="1" max="2" min="2" style="12" width="24.1640625"/>
-    <col customWidth="1" max="3" min="3" style="12" width="24.6640625"/>
+    <col min="1" max="1" width="18" style="12" customWidth="1"/>
+    <col min="2" max="2" width="24.1640625" style="12" customWidth="1"/>
+    <col min="3" max="3" width="24.6640625" style="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="33" r="1" s="12" spans="1:3">
+    <row r="1" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="8" t="s">
+    </row>
+    <row r="3" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row customHeight="1" ht="19" r="2" s="12" spans="1:3">
-      <c r="A2" s="9" t="s">
+      <c r="B3" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="C3" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="10" t="s">
+    </row>
+    <row r="4" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="11"/>
+      <c r="B4" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="11"/>
+      <c r="B5" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="10" t="s">
         <v>26</v>
       </c>
     </row>
-    <row customHeight="1" ht="19" r="3" s="12" spans="1:3">
-      <c r="A3" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" s="10" t="s">
+    <row r="6" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="11"/>
+      <c r="B6" s="10" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row customHeight="1" ht="19" r="4" s="12" spans="1:3">
-      <c r="A4" s="11" t="n"/>
-      <c r="B4" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" s="10" t="s">
+      <c r="C6" s="9"/>
+    </row>
+    <row r="7" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="11"/>
+      <c r="B7" s="10" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row customHeight="1" ht="19" r="5" s="12" spans="1:3">
-      <c r="A5" s="11" t="n"/>
-      <c r="B5" s="10" t="s">
+      <c r="C7" s="9"/>
+    </row>
+    <row r="8" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="11"/>
+      <c r="B8" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C8" s="9"/>
+    </row>
+    <row r="9" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="11"/>
+      <c r="B9" s="10" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row customHeight="1" ht="19" r="6" s="12" spans="1:3">
-      <c r="A6" s="11" t="n"/>
-      <c r="B6" s="10" t="s">
+      <c r="C9" s="9"/>
+    </row>
+    <row r="10" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="11"/>
+      <c r="B10" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="9"/>
+    </row>
+    <row r="11" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="11"/>
+      <c r="B11" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="9" t="n"/>
-    </row>
-    <row customHeight="1" ht="19" r="7" s="12" spans="1:3">
-      <c r="A7" s="11" t="n"/>
-      <c r="B7" s="10" t="s">
+      <c r="C11" s="9"/>
+    </row>
+    <row r="12" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="11"/>
+      <c r="B12" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="9" t="n"/>
-    </row>
-    <row customHeight="1" ht="19" r="8" s="12" spans="1:3">
-      <c r="A8" s="11" t="n"/>
-      <c r="B8" s="10" t="s">
+      <c r="C12" s="9"/>
+    </row>
+    <row r="13" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="11"/>
+      <c r="B13" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="9" t="n"/>
-    </row>
-    <row customHeight="1" ht="19" r="9" s="12" spans="1:3">
-      <c r="A9" s="11" t="n"/>
-      <c r="B9" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="C9" s="9" t="n"/>
-    </row>
-    <row customHeight="1" ht="19" r="10" s="12" spans="1:3">
-      <c r="A10" s="11" t="n"/>
-      <c r="B10" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="C10" s="9" t="n"/>
-    </row>
-    <row customHeight="1" ht="19" r="11" s="12" spans="1:3">
-      <c r="A11" s="11" t="n"/>
-      <c r="B11" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="C11" s="9" t="n"/>
-    </row>
-    <row customHeight="1" ht="19" r="12" s="12" spans="1:3">
-      <c r="A12" s="11" t="n"/>
-      <c r="B12" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="C12" s="9" t="n"/>
-    </row>
-    <row customHeight="1" ht="19" r="13" s="12" spans="1:3">
-      <c r="A13" s="11" t="n"/>
-      <c r="B13" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="C13" s="9" t="n"/>
-    </row>
-    <row customHeight="1" ht="19" r="14" s="12" spans="1:3">
-      <c r="B14" s="7" t="n"/>
-      <c r="C14" s="7" t="n"/>
-    </row>
-    <row customHeight="1" ht="19" r="15" s="12" spans="1:3">
-      <c r="B15" s="7" t="n"/>
-      <c r="C15" s="7" t="n"/>
+      <c r="C13" s="9"/>
+    </row>
+    <row r="14" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+    </row>
+    <row r="15" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added ability to run saline scenarios using the SAR input parameter.
</commit_message>
<xml_diff>
--- a/RHEM_template.xlsx
+++ b/RHEM_template.xlsx
@@ -8,23 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gerardo/my/Projects/RHEM/RHEM_batch_app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{975435A8-627A-CB43-BE78-D1159654D3D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C047433-7BCA-5543-BF67-2A10C5A3BBF0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="51200" windowHeight="28360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="51200" windowHeight="28280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs" sheetId="1" r:id="rId1"/>
     <sheet name="Lookup Tables" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="Uniform">Inputs!$H$2</definedName>
+    <definedName name="Uniform">Inputs!$I$2</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
   <si>
     <t>Scenario Name</t>
   </si>
@@ -32,109 +32,118 @@
     <t>Scenario Description</t>
   </si>
   <si>
+    <t>Units (metric only)</t>
+  </si>
+  <si>
+    <t>State ID</t>
+  </si>
+  <si>
+    <t>Climate Station ID</t>
+  </si>
+  <si>
+    <t>Soil Texture</t>
+  </si>
+  <si>
+    <t>SAR</t>
+  </si>
+  <si>
+    <t>Slope Length (meters)</t>
+  </si>
+  <si>
+    <t>Slope Shape (Uniform, S-Shaped, Convex, Concave)</t>
+  </si>
+  <si>
+    <t>Slope Steepness ( % )</t>
+  </si>
+  <si>
+    <t>Bunch Grass ( % )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forbs/Annuals ( %) </t>
+  </si>
+  <si>
+    <t>Shrubs ( % )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sod Grass (%) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Basal Plant Cover ( % ) </t>
+  </si>
+  <si>
+    <t>Rock Cover ( % )</t>
+  </si>
+  <si>
+    <t>Litter Cover  ( % )</t>
+  </si>
+  <si>
+    <t>Biological Crusts Cover            ( % )</t>
+  </si>
+  <si>
+    <t>Avg Precipitation (mm/year)</t>
+  </si>
+  <si>
+    <t>Avg Runoff (mm/year)</t>
+  </si>
+  <si>
+    <t>Avg Soil Loss (ton/ha/year)</t>
+  </si>
+  <si>
+    <t>Avg SY (ton/ha/year)</t>
+  </si>
+  <si>
+    <t>TDS (ton/ha/year)</t>
+  </si>
+  <si>
+    <t>NOTE:  Please use the  "Lookup Tables" tab to get the possible values for Units, Soil Texture, and Slope Shape.  To find the climate station IDs, visit the Climate Station section of the RHEM Web Tool: https://apps.tucson.ars.ag.gov/rhem</t>
+  </si>
+  <si>
+    <t>CO</t>
+  </si>
+  <si>
+    <t>053488</t>
+  </si>
+  <si>
+    <t>Silty Clay Loam</t>
+  </si>
+  <si>
+    <t>Concave</t>
+  </si>
+  <si>
     <t>Units</t>
   </si>
   <si>
-    <t>State ID</t>
-  </si>
-  <si>
-    <t>Climate Station ID</t>
-  </si>
-  <si>
-    <t>Soil Texture</t>
-  </si>
-  <si>
-    <t>Slope Length (meters)</t>
-  </si>
-  <si>
-    <t>Slope Shape (Uniform, S-Shaped, Convex, Concave)</t>
-  </si>
-  <si>
-    <t>Slope Steepness ( % )</t>
-  </si>
-  <si>
-    <t>Bunch Grass ( % )</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Forbs/Annuals ( %) </t>
-  </si>
-  <si>
-    <t>Shrubs ( % )</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sod Grass (%) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Basal Plant Cover ( % ) </t>
-  </si>
-  <si>
-    <t>Rock Cover ( % )</t>
-  </si>
-  <si>
-    <t>Litter Cover  ( % )</t>
-  </si>
-  <si>
-    <t>Biological Crusts Cover            ( % )</t>
-  </si>
-  <si>
-    <t>Avg Precipitation (mm/year)</t>
-  </si>
-  <si>
-    <t>Avg Runoff (mm/year)</t>
-  </si>
-  <si>
-    <t>Avg Soil Loss (ton/ha/year)</t>
-  </si>
-  <si>
-    <t>Avg SY (ton/ha/year)</t>
-  </si>
-  <si>
-    <t>NOTE:  Please use the  "Lookup Tables" tab to get the possible values for Units, Soil Texture, and Slope Shape.  To find the climate station IDs, visit the Climate Station section of the RHEM Web Tool: https://apps.tucson.ars.ag.gov/rhem</t>
-  </si>
-  <si>
-    <t>CO</t>
-  </si>
-  <si>
-    <t>053488</t>
-  </si>
-  <si>
-    <t>Silty Clay Loam</t>
-  </si>
-  <si>
-    <t>Concave</t>
+    <t>Soil Types</t>
+  </si>
+  <si>
+    <t>Slope Shape</t>
+  </si>
+  <si>
+    <t>1 (Metric)</t>
+  </si>
+  <si>
+    <t>Sand</t>
+  </si>
+  <si>
+    <t>Uniform</t>
+  </si>
+  <si>
+    <t>2 (English)</t>
+  </si>
+  <si>
+    <t>Loamy Sand</t>
+  </si>
+  <si>
+    <t>Convex</t>
+  </si>
+  <si>
+    <t>Sandy Loam</t>
+  </si>
+  <si>
+    <t>Loam</t>
   </si>
   <si>
     <t>S-Shaped</t>
-  </si>
-  <si>
-    <t>Soil Types</t>
-  </si>
-  <si>
-    <t>Slope Shape</t>
-  </si>
-  <si>
-    <t>1 (Metric)</t>
-  </si>
-  <si>
-    <t>Sand</t>
-  </si>
-  <si>
-    <t>Uniform</t>
-  </si>
-  <si>
-    <t>2 (English)</t>
-  </si>
-  <si>
-    <t>Loamy Sand</t>
-  </si>
-  <si>
-    <t>Convex</t>
-  </si>
-  <si>
-    <t>Sandy Loam</t>
-  </si>
-  <si>
-    <t>Loam</t>
   </si>
   <si>
     <t>Silt Loam</t>
@@ -269,7 +278,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -307,7 +316,6 @@
     <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -625,32 +633,34 @@
   <dimension ref="A1:AA3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="T2" sqref="T2:X3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.1640625" style="12" customWidth="1"/>
     <col min="2" max="2" width="22" style="12" customWidth="1"/>
-    <col min="3" max="3" width="6.1640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" style="12" customWidth="1"/>
     <col min="4" max="4" width="10.83203125" style="12" customWidth="1"/>
     <col min="5" max="5" width="12.6640625" style="13" customWidth="1"/>
     <col min="6" max="6" width="14.83203125" style="12" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.5" style="12" customWidth="1"/>
-    <col min="9" max="9" width="11.5" style="12" customWidth="1"/>
-    <col min="10" max="10" width="11.83203125" style="12" customWidth="1"/>
-    <col min="11" max="11" width="15.83203125" style="12" customWidth="1"/>
-    <col min="12" max="12" width="8" style="12" customWidth="1"/>
-    <col min="13" max="13" width="7.83203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.33203125" style="12" customWidth="1"/>
-    <col min="15" max="15" width="7.1640625" style="12" customWidth="1"/>
-    <col min="16" max="16" width="8" style="12" customWidth="1"/>
-    <col min="17" max="17" width="11.33203125" style="12" customWidth="1"/>
-    <col min="19" max="19" width="21" style="12" customWidth="1"/>
-    <col min="20" max="20" width="16.83203125" style="12" customWidth="1"/>
-    <col min="21" max="21" width="18.33203125" style="12" customWidth="1"/>
-    <col min="22" max="22" width="16.6640625" style="12" customWidth="1"/>
+    <col min="7" max="7" width="7.83203125" style="12" customWidth="1"/>
+    <col min="8" max="8" width="13.33203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.5" style="12" customWidth="1"/>
+    <col min="10" max="10" width="11.5" style="12" customWidth="1"/>
+    <col min="11" max="11" width="11.83203125" style="12" customWidth="1"/>
+    <col min="12" max="12" width="15.83203125" style="12" customWidth="1"/>
+    <col min="13" max="13" width="8" style="12" customWidth="1"/>
+    <col min="14" max="14" width="7.83203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.33203125" style="12" customWidth="1"/>
+    <col min="16" max="16" width="7.1640625" style="12" customWidth="1"/>
+    <col min="17" max="17" width="8" style="12" customWidth="1"/>
+    <col min="18" max="18" width="11.33203125" style="12" customWidth="1"/>
+    <col min="20" max="20" width="21" style="12" customWidth="1"/>
+    <col min="21" max="21" width="16.83203125" style="12" customWidth="1"/>
+    <col min="22" max="22" width="18.33203125" style="12" customWidth="1"/>
+    <col min="23" max="23" width="16.6640625" style="12" customWidth="1"/>
+    <col min="24" max="24" width="16" style="12" customWidth="1"/>
     <col min="25" max="25" width="108" style="12" customWidth="1"/>
   </cols>
   <sheetData>
@@ -661,7 +671,7 @@
       <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="5" t="s">
@@ -706,7 +716,7 @@
       <c r="Q1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="R1" s="3" t="s">
         <v>17</v>
       </c>
       <c r="T1" s="2" t="s">
@@ -718,53 +728,57 @@
       <c r="V1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
+      <c r="W1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="Y1" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="Z1" s="1"/>
       <c r="AA1" s="1"/>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A2" s="14">
+      <c r="A2" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="15">
-        <v>3</v>
-      </c>
       <c r="C2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="G2">
+        <v>25</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" s="16">
+        <v>0</v>
+      </c>
+      <c r="H2">
         <v>50</v>
       </c>
-      <c r="H2" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="I2" s="15">
-        <v>15.80000019073486</v>
+      <c r="I2" s="16" t="s">
+        <v>27</v>
       </c>
       <c r="J2" s="15">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="K2" s="15">
         <v>0</v>
       </c>
       <c r="L2" s="15">
+        <v>0</v>
+      </c>
+      <c r="M2" s="15">
         <v>20</v>
-      </c>
-      <c r="M2" s="15">
-        <v>0</v>
       </c>
       <c r="N2" s="15">
         <v>0</v>
@@ -773,22 +787,26 @@
         <v>0</v>
       </c>
       <c r="P2" s="15">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="15">
         <v>30</v>
       </c>
-      <c r="Q2" s="15">
+      <c r="R2" s="15">
         <v>0</v>
       </c>
-      <c r="S2"/>
       <c r="T2"/>
       <c r="U2"/>
       <c r="V2"/>
+      <c r="W2"/>
+      <c r="X2"/>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A3" s="14"/>
       <c r="B3" s="15"/>
       <c r="F3" s="15"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="I3" s="16"/>
       <c r="J3" s="15"/>
       <c r="K3" s="15"/>
       <c r="L3" s="15"/>
@@ -797,6 +815,7 @@
       <c r="O3" s="15"/>
       <c r="P3" s="15"/>
       <c r="Q3" s="15"/>
+      <c r="R3" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -821,108 +840,108 @@
   <sheetData>
     <row r="1" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
       <c r="B4" s="10" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11"/>
       <c r="B5" s="10" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11"/>
       <c r="B6" s="10" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C6" s="9"/>
     </row>
     <row r="7" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="11"/>
       <c r="B7" s="10" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C7" s="9"/>
     </row>
     <row r="8" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11"/>
       <c r="B8" s="10" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C8" s="9"/>
     </row>
     <row r="9" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11"/>
       <c r="B9" s="10" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C9" s="9"/>
     </row>
     <row r="10" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11"/>
       <c r="B10" s="10" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C10" s="9"/>
     </row>
     <row r="11" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="11"/>
       <c r="B11" s="10" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C11" s="9"/>
     </row>
     <row r="12" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11"/>
       <c r="B12" s="10" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C12" s="9"/>
     </row>
     <row r="13" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="11"/>
       <c r="B13" s="10" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C13" s="9"/>
     </row>

</xml_diff>

<commit_message>
Updated note with kmz for international stations
</commit_message>
<xml_diff>
--- a/RHEM_template.xlsx
+++ b/RHEM_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gerardo/my/Projects/RHEM/RHEM_batch_app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C047433-7BCA-5543-BF67-2A10C5A3BBF0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{244772E7-8D38-F441-996E-16197167DB00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="51200" windowHeight="28280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,14 +17,14 @@
     <sheet name="Lookup Tables" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="Uniform">Inputs!$I$2</definedName>
+    <definedName name="Uniform">Inputs!$I$33</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="49">
   <si>
     <t>Scenario Name</t>
   </si>
@@ -95,13 +95,10 @@
     <t>TDS (ton/ha/year)</t>
   </si>
   <si>
-    <t>NOTE:  Please use the  "Lookup Tables" tab to get the possible values for Units, Soil Texture, and Slope Shape.  To find the climate station IDs, visit the Climate Station section of the RHEM Web Tool: https://apps.tucson.ars.ag.gov/rhem</t>
-  </si>
-  <si>
-    <t>CO</t>
-  </si>
-  <si>
-    <t>053488</t>
+    <t>INTL_BR</t>
+  </si>
+  <si>
+    <t>BR002156000</t>
   </si>
   <si>
     <t>Silty Clay Loam</t>
@@ -110,6 +107,12 @@
     <t>Concave</t>
   </si>
   <si>
+    <t>UT</t>
+  </si>
+  <si>
+    <t>423611</t>
+  </si>
+  <si>
     <t>Units</t>
   </si>
   <si>
@@ -165,6 +168,9 @@
   </si>
   <si>
     <t>Clay</t>
+  </si>
+  <si>
+    <t>NOTE:  Please use the  "Lookup Tables" tab to get the possible values for Units, Soil Texture, and Slope Shape.  To find the climate station IDs, visit the Climate Station section of the RHEM Web Tool: https://apps.tucson.ars.ag.gov/rhem.  For the listing of international stations, you can download this KMZ layer: http://apps.tucson.ars.ag.gov/rhem/assets/kmz/International_CLIGEN_stations.kmz For State ID, if using an international station, precede the the country code with "INTL_" i.e. INTL_US</t>
   </si>
 </sst>
 </file>
@@ -630,10 +636,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA3"/>
+  <dimension ref="A1:AA39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T2" sqref="T2:X3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -664,7 +670,7 @@
     <col min="25" max="25" width="108" style="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="108" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" ht="179" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -735,7 +741,7 @@
         <v>22</v>
       </c>
       <c r="Y1" s="4" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="Z1" s="1"/>
       <c r="AA1" s="1"/>
@@ -751,13 +757,13 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="F2" s="16" t="s">
         <v>25</v>
-      </c>
-      <c r="F2" s="16" t="s">
-        <v>26</v>
       </c>
       <c r="G2" s="16">
         <v>0</v>
@@ -766,7 +772,7 @@
         <v>50</v>
       </c>
       <c r="I2" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J2" s="15">
         <v>15</v>
@@ -802,20 +808,222 @@
       <c r="X2"/>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A3" s="14"/>
-      <c r="B3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="15"/>
-      <c r="L3" s="15"/>
-      <c r="M3" s="15"/>
-      <c r="N3" s="15"/>
-      <c r="O3" s="15"/>
-      <c r="P3" s="15"/>
-      <c r="Q3" s="15"/>
-      <c r="R3" s="15"/>
+      <c r="A3" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="16">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>50</v>
+      </c>
+      <c r="I3" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" s="15">
+        <v>15</v>
+      </c>
+      <c r="K3" s="15">
+        <v>0</v>
+      </c>
+      <c r="L3" s="15">
+        <v>0</v>
+      </c>
+      <c r="M3" s="15">
+        <v>20</v>
+      </c>
+      <c r="N3" s="15">
+        <v>0</v>
+      </c>
+      <c r="O3" s="15">
+        <v>0</v>
+      </c>
+      <c r="P3" s="15">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="15">
+        <v>30</v>
+      </c>
+      <c r="R3" s="15">
+        <v>0</v>
+      </c>
+      <c r="T3"/>
+      <c r="U3"/>
+      <c r="V3"/>
+      <c r="W3"/>
+      <c r="X3"/>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A4" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="15"/>
+      <c r="C4"/>
+      <c r="D4"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="15"/>
+      <c r="M4" s="15"/>
+      <c r="N4" s="15"/>
+      <c r="O4" s="15"/>
+      <c r="P4" s="15"/>
+      <c r="Q4" s="15"/>
+      <c r="R4" s="15"/>
+      <c r="T4"/>
+      <c r="U4"/>
+      <c r="V4"/>
+      <c r="W4"/>
+      <c r="X4"/>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A5" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="15"/>
+      <c r="C5"/>
+      <c r="D5"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="15"/>
+      <c r="O5" s="15"/>
+      <c r="P5" s="15"/>
+      <c r="Q5" s="15"/>
+      <c r="R5" s="15"/>
+      <c r="T5"/>
+      <c r="U5"/>
+      <c r="V5"/>
+      <c r="W5"/>
+      <c r="X5"/>
+    </row>
+    <row r="33" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A33" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B33" s="15"/>
+      <c r="C33"/>
+      <c r="D33"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="16"/>
+      <c r="H33"/>
+      <c r="I33" s="16"/>
+      <c r="J33" s="15"/>
+      <c r="K33" s="15"/>
+      <c r="L33" s="15"/>
+      <c r="M33" s="15"/>
+      <c r="N33" s="15"/>
+      <c r="O33" s="15"/>
+      <c r="P33" s="15"/>
+      <c r="Q33" s="15"/>
+      <c r="R33" s="15"/>
+      <c r="T33"/>
+      <c r="U33"/>
+      <c r="V33"/>
+      <c r="W33"/>
+      <c r="X33"/>
+      <c r="Y33"/>
+    </row>
+    <row r="35" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A35" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B35" s="15"/>
+      <c r="C35"/>
+      <c r="D35"/>
+      <c r="F35" s="16"/>
+      <c r="G35" s="16"/>
+      <c r="H35"/>
+      <c r="I35" s="16"/>
+      <c r="J35" s="15"/>
+      <c r="K35" s="15"/>
+      <c r="L35" s="15"/>
+      <c r="M35" s="15"/>
+      <c r="N35" s="15"/>
+      <c r="O35" s="15"/>
+      <c r="P35" s="15"/>
+      <c r="Q35" s="15"/>
+      <c r="R35" s="15"/>
+      <c r="T35"/>
+      <c r="U35"/>
+      <c r="V35"/>
+      <c r="W35"/>
+      <c r="X35"/>
+      <c r="Y35"/>
+    </row>
+    <row r="37" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A37" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B37" s="15"/>
+      <c r="C37"/>
+      <c r="D37"/>
+      <c r="F37" s="16"/>
+      <c r="G37" s="16"/>
+      <c r="H37"/>
+      <c r="I37" s="16"/>
+      <c r="J37" s="15"/>
+      <c r="K37" s="15"/>
+      <c r="L37" s="15"/>
+      <c r="M37" s="15"/>
+      <c r="N37" s="15"/>
+      <c r="O37" s="15"/>
+      <c r="P37" s="15"/>
+      <c r="Q37" s="15"/>
+      <c r="R37" s="15"/>
+      <c r="T37"/>
+      <c r="U37"/>
+      <c r="V37"/>
+      <c r="W37"/>
+      <c r="X37"/>
+      <c r="Y37"/>
+    </row>
+    <row r="39" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B39" s="15"/>
+      <c r="C39"/>
+      <c r="D39"/>
+      <c r="F39" s="16"/>
+      <c r="G39" s="16"/>
+      <c r="H39"/>
+      <c r="I39" s="16"/>
+      <c r="J39" s="15"/>
+      <c r="K39" s="15"/>
+      <c r="L39" s="15"/>
+      <c r="M39" s="15"/>
+      <c r="N39" s="15"/>
+      <c r="O39" s="15"/>
+      <c r="P39" s="15"/>
+      <c r="Q39" s="15"/>
+      <c r="R39" s="15"/>
+      <c r="T39"/>
+      <c r="U39"/>
+      <c r="V39"/>
+      <c r="W39"/>
+      <c r="X39"/>
+      <c r="Y39"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -840,108 +1048,108 @@
   <sheetData>
     <row r="1" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
       <c r="B4" s="10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11"/>
       <c r="B5" s="10" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11"/>
       <c r="B6" s="10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C6" s="9"/>
     </row>
     <row r="7" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="11"/>
       <c r="B7" s="10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C7" s="9"/>
     </row>
     <row r="8" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11"/>
       <c r="B8" s="10" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C8" s="9"/>
     </row>
     <row r="9" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11"/>
       <c r="B9" s="10" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C9" s="9"/>
     </row>
     <row r="10" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11"/>
       <c r="B10" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C10" s="9"/>
     </row>
     <row r="11" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="11"/>
       <c r="B11" s="10" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C11" s="9"/>
     </row>
     <row r="12" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11"/>
       <c r="B12" s="10" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C12" s="9"/>
     </row>
     <row r="13" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="11"/>
       <c r="B13" s="10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C13" s="9"/>
     </row>

</xml_diff>

<commit_message>
Added async support to run scenarios in parallel
</commit_message>
<xml_diff>
--- a/RHEM_template.xlsx
+++ b/RHEM_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gerardo/my/Projects/RHEM/RHEM_batch_app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{244772E7-8D38-F441-996E-16197167DB00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3F8A690-922A-F246-A208-4072923D4BCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="51200" windowHeight="28280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="49">
   <si>
     <t>Scenario Name</t>
   </si>
@@ -95,6 +95,15 @@
     <t>TDS (ton/ha/year)</t>
   </si>
   <si>
+    <t>NOTE:  Please use the  "Lookup Tables" tab to get the possible values for Units, Soil Texture, and Slope Shape.  To find the climate station IDs, visit the Climate Station section of the RHEM Web Tool: https://apps.tucson.ars.ag.gov/rhem.  For the listing of international stations, you can download this KMZ layer: http://apps.tucson.ars.ag.gov/rhem/assets/kmz/International_CLIGEN_stations.kmz For State ID, if using an international station, precede the the country code with "INTL_" i.e. INTL_US</t>
+  </si>
+  <si>
+    <t>Scenario Name 1</t>
+  </si>
+  <si>
+    <t>Scenario Description 1</t>
+  </si>
+  <si>
     <t>INTL_BR</t>
   </si>
   <si>
@@ -107,12 +116,6 @@
     <t>Concave</t>
   </si>
   <si>
-    <t>UT</t>
-  </si>
-  <si>
-    <t>423611</t>
-  </si>
-  <si>
     <t>Units</t>
   </si>
   <si>
@@ -168,9 +171,6 @@
   </si>
   <si>
     <t>Clay</t>
-  </si>
-  <si>
-    <t>NOTE:  Please use the  "Lookup Tables" tab to get the possible values for Units, Soil Texture, and Slope Shape.  To find the climate station IDs, visit the Climate Station section of the RHEM Web Tool: https://apps.tucson.ars.ag.gov/rhem.  For the listing of international stations, you can download this KMZ layer: http://apps.tucson.ars.ag.gov/rhem/assets/kmz/International_CLIGEN_stations.kmz For State ID, if using an international station, precede the the country code with "INTL_" i.e. INTL_US</t>
   </si>
 </sst>
 </file>
@@ -638,8 +638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="X14" sqref="X14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -741,29 +741,29 @@
         <v>22</v>
       </c>
       <c r="Y1" s="4" t="s">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="Z1" s="1"/>
       <c r="AA1" s="1"/>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="G2" s="16">
         <v>0</v>
@@ -772,7 +772,7 @@
         <v>50</v>
       </c>
       <c r="I2" s="16" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="J2" s="15">
         <v>15</v>
@@ -808,60 +808,23 @@
       <c r="X2"/>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A3" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="G3" s="16">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>50</v>
-      </c>
-      <c r="I3" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="J3" s="15">
-        <v>15</v>
-      </c>
-      <c r="K3" s="15">
-        <v>0</v>
-      </c>
-      <c r="L3" s="15">
-        <v>0</v>
-      </c>
-      <c r="M3" s="15">
-        <v>20</v>
-      </c>
-      <c r="N3" s="15">
-        <v>0</v>
-      </c>
-      <c r="O3" s="15">
-        <v>0</v>
-      </c>
-      <c r="P3" s="15">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="15">
-        <v>30</v>
-      </c>
-      <c r="R3" s="15">
-        <v>0</v>
-      </c>
+      <c r="A3" s="14"/>
+      <c r="B3" s="15"/>
+      <c r="C3"/>
+      <c r="D3"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="15"/>
+      <c r="O3" s="15"/>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="15"/>
+      <c r="R3" s="15"/>
       <c r="T3"/>
       <c r="U3"/>
       <c r="V3"/>
@@ -869,9 +832,7 @@
       <c r="X3"/>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A4" s="14" t="s">
-        <v>0</v>
-      </c>
+      <c r="A4" s="14"/>
       <c r="B4" s="15"/>
       <c r="C4"/>
       <c r="D4"/>
@@ -895,9 +856,7 @@
       <c r="X4"/>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A5" s="14" t="s">
-        <v>0</v>
-      </c>
+      <c r="A5" s="14"/>
       <c r="B5" s="15"/>
       <c r="C5"/>
       <c r="D5"/>
@@ -920,16 +879,395 @@
       <c r="W5"/>
       <c r="X5"/>
     </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A33" s="14" t="s">
-        <v>0</v>
-      </c>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A6" s="14"/>
+      <c r="B6" s="15"/>
+      <c r="C6"/>
+      <c r="D6"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="15"/>
+      <c r="O6" s="15"/>
+      <c r="P6" s="15"/>
+      <c r="Q6" s="15"/>
+      <c r="R6" s="15"/>
+      <c r="T6"/>
+      <c r="U6"/>
+      <c r="V6"/>
+      <c r="W6"/>
+      <c r="X6"/>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A7" s="14"/>
+      <c r="B7" s="15"/>
+      <c r="C7"/>
+      <c r="D7"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="15"/>
+      <c r="N7" s="15"/>
+      <c r="O7" s="15"/>
+      <c r="P7" s="15"/>
+      <c r="Q7" s="15"/>
+      <c r="R7" s="15"/>
+      <c r="T7"/>
+      <c r="U7"/>
+      <c r="V7"/>
+      <c r="W7"/>
+      <c r="X7"/>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A8" s="14"/>
+      <c r="B8" s="15"/>
+      <c r="C8"/>
+      <c r="D8"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="15"/>
+      <c r="O8" s="15"/>
+      <c r="P8" s="15"/>
+      <c r="Q8" s="15"/>
+      <c r="R8" s="15"/>
+      <c r="T8"/>
+      <c r="U8"/>
+      <c r="V8"/>
+      <c r="W8"/>
+      <c r="X8"/>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A9" s="14"/>
+      <c r="B9" s="15"/>
+      <c r="C9"/>
+      <c r="D9"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="15"/>
+      <c r="N9" s="15"/>
+      <c r="O9" s="15"/>
+      <c r="P9" s="15"/>
+      <c r="Q9" s="15"/>
+      <c r="R9" s="15"/>
+      <c r="T9"/>
+      <c r="U9"/>
+      <c r="V9"/>
+      <c r="W9"/>
+      <c r="X9"/>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A10" s="14"/>
+      <c r="B10" s="15"/>
+      <c r="C10"/>
+      <c r="D10"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="15"/>
+      <c r="M10" s="15"/>
+      <c r="N10" s="15"/>
+      <c r="O10" s="15"/>
+      <c r="P10" s="15"/>
+      <c r="Q10" s="15"/>
+      <c r="R10" s="15"/>
+      <c r="T10"/>
+      <c r="U10"/>
+      <c r="V10"/>
+      <c r="W10"/>
+      <c r="X10"/>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A11" s="14"/>
+      <c r="B11" s="15"/>
+      <c r="C11"/>
+      <c r="D11"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="15"/>
+      <c r="N11" s="15"/>
+      <c r="O11" s="15"/>
+      <c r="P11" s="15"/>
+      <c r="Q11" s="15"/>
+      <c r="R11" s="15"/>
+      <c r="T11"/>
+      <c r="U11"/>
+      <c r="V11"/>
+      <c r="W11"/>
+      <c r="X11"/>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A12" s="14"/>
+      <c r="B12" s="15"/>
+      <c r="C12"/>
+      <c r="D12"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
+      <c r="L12" s="15"/>
+      <c r="M12" s="15"/>
+      <c r="N12" s="15"/>
+      <c r="O12" s="15"/>
+      <c r="P12" s="15"/>
+      <c r="Q12" s="15"/>
+      <c r="R12" s="15"/>
+      <c r="T12"/>
+      <c r="U12"/>
+      <c r="V12"/>
+      <c r="W12"/>
+      <c r="X12"/>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A13" s="14"/>
+      <c r="B13" s="15"/>
+      <c r="C13"/>
+      <c r="D13"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="15"/>
+      <c r="M13" s="15"/>
+      <c r="N13" s="15"/>
+      <c r="O13" s="15"/>
+      <c r="P13" s="15"/>
+      <c r="Q13" s="15"/>
+      <c r="R13" s="15"/>
+      <c r="T13"/>
+      <c r="U13"/>
+      <c r="V13"/>
+      <c r="W13"/>
+      <c r="X13"/>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A14" s="14"/>
+      <c r="B14" s="15"/>
+      <c r="C14"/>
+      <c r="D14"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14"/>
+      <c r="I14" s="16"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="15"/>
+      <c r="M14" s="15"/>
+      <c r="N14" s="15"/>
+      <c r="O14" s="15"/>
+      <c r="P14" s="15"/>
+      <c r="Q14" s="15"/>
+      <c r="R14" s="15"/>
+      <c r="T14"/>
+      <c r="U14"/>
+      <c r="V14"/>
+      <c r="W14"/>
+      <c r="X14"/>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A15" s="14"/>
+      <c r="B15" s="15"/>
+      <c r="C15"/>
+      <c r="D15"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="15"/>
+      <c r="L15" s="15"/>
+      <c r="M15" s="15"/>
+      <c r="N15" s="15"/>
+      <c r="O15" s="15"/>
+      <c r="P15" s="15"/>
+      <c r="Q15" s="15"/>
+      <c r="R15" s="15"/>
+      <c r="T15"/>
+      <c r="U15"/>
+      <c r="V15"/>
+      <c r="W15"/>
+      <c r="X15"/>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A16" s="14"/>
+      <c r="B16" s="15"/>
+      <c r="C16"/>
+      <c r="D16"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
+      <c r="H16"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="15"/>
+      <c r="L16" s="15"/>
+      <c r="M16" s="15"/>
+      <c r="N16" s="15"/>
+      <c r="O16" s="15"/>
+      <c r="P16" s="15"/>
+      <c r="Q16" s="15"/>
+      <c r="R16" s="15"/>
+      <c r="T16"/>
+      <c r="U16"/>
+      <c r="V16"/>
+      <c r="W16"/>
+      <c r="X16"/>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A17" s="14"/>
+      <c r="B17" s="15"/>
+      <c r="C17"/>
+      <c r="D17"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+      <c r="H17"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="15"/>
+      <c r="L17" s="15"/>
+      <c r="M17" s="15"/>
+      <c r="N17" s="15"/>
+      <c r="O17" s="15"/>
+      <c r="P17" s="15"/>
+      <c r="Q17" s="15"/>
+      <c r="R17" s="15"/>
+      <c r="T17"/>
+      <c r="U17"/>
+      <c r="V17"/>
+      <c r="W17"/>
+      <c r="X17"/>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A18" s="14"/>
+      <c r="B18" s="15"/>
+      <c r="C18"/>
+      <c r="D18"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+      <c r="H18"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="15"/>
+      <c r="L18" s="15"/>
+      <c r="M18" s="15"/>
+      <c r="N18" s="15"/>
+      <c r="O18" s="15"/>
+      <c r="P18" s="15"/>
+      <c r="Q18" s="15"/>
+      <c r="R18" s="15"/>
+      <c r="T18"/>
+      <c r="U18"/>
+      <c r="V18"/>
+      <c r="W18"/>
+      <c r="X18"/>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A19" s="14"/>
+      <c r="B19" s="15"/>
+      <c r="C19"/>
+      <c r="D19"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
+      <c r="H19"/>
+      <c r="I19" s="16"/>
+      <c r="J19" s="15"/>
+      <c r="K19" s="15"/>
+      <c r="L19" s="15"/>
+      <c r="M19" s="15"/>
+      <c r="N19" s="15"/>
+      <c r="O19" s="15"/>
+      <c r="P19" s="15"/>
+      <c r="Q19" s="15"/>
+      <c r="R19" s="15"/>
+      <c r="T19"/>
+      <c r="U19"/>
+      <c r="V19"/>
+      <c r="W19"/>
+      <c r="X19"/>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A20" s="14"/>
+      <c r="B20" s="15"/>
+      <c r="C20"/>
+      <c r="D20"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20"/>
+      <c r="I20" s="16"/>
+      <c r="J20" s="15"/>
+      <c r="K20" s="15"/>
+      <c r="L20" s="15"/>
+      <c r="M20" s="15"/>
+      <c r="N20" s="15"/>
+      <c r="O20" s="15"/>
+      <c r="P20" s="15"/>
+      <c r="Q20" s="15"/>
+      <c r="R20" s="15"/>
+      <c r="T20"/>
+      <c r="U20"/>
+      <c r="V20"/>
+      <c r="W20"/>
+      <c r="X20"/>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A21" s="14"/>
+      <c r="B21" s="15"/>
+      <c r="C21"/>
+      <c r="D21"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16"/>
+      <c r="H21"/>
+      <c r="I21" s="16"/>
+      <c r="J21" s="15"/>
+      <c r="K21" s="15"/>
+      <c r="L21" s="15"/>
+      <c r="M21" s="15"/>
+      <c r="N21" s="15"/>
+      <c r="O21" s="15"/>
+      <c r="P21" s="15"/>
+      <c r="Q21" s="15"/>
+      <c r="R21" s="15"/>
+      <c r="T21"/>
+      <c r="U21"/>
+      <c r="V21"/>
+      <c r="W21"/>
+      <c r="X21"/>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A33" s="14"/>
       <c r="B33" s="15"/>
-      <c r="C33"/>
-      <c r="D33"/>
       <c r="F33" s="16"/>
       <c r="G33" s="16"/>
-      <c r="H33"/>
       <c r="I33" s="16"/>
       <c r="J33" s="15"/>
       <c r="K33" s="15"/>
@@ -940,23 +1278,12 @@
       <c r="P33" s="15"/>
       <c r="Q33" s="15"/>
       <c r="R33" s="15"/>
-      <c r="T33"/>
-      <c r="U33"/>
-      <c r="V33"/>
-      <c r="W33"/>
-      <c r="X33"/>
-      <c r="Y33"/>
-    </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A35" s="14" t="s">
-        <v>0</v>
-      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A35" s="14"/>
       <c r="B35" s="15"/>
-      <c r="C35"/>
-      <c r="D35"/>
       <c r="F35" s="16"/>
       <c r="G35" s="16"/>
-      <c r="H35"/>
       <c r="I35" s="16"/>
       <c r="J35" s="15"/>
       <c r="K35" s="15"/>
@@ -967,23 +1294,12 @@
       <c r="P35" s="15"/>
       <c r="Q35" s="15"/>
       <c r="R35" s="15"/>
-      <c r="T35"/>
-      <c r="U35"/>
-      <c r="V35"/>
-      <c r="W35"/>
-      <c r="X35"/>
-      <c r="Y35"/>
-    </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A37" s="14" t="s">
-        <v>0</v>
-      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A37" s="14"/>
       <c r="B37" s="15"/>
-      <c r="C37"/>
-      <c r="D37"/>
       <c r="F37" s="16"/>
       <c r="G37" s="16"/>
-      <c r="H37"/>
       <c r="I37" s="16"/>
       <c r="J37" s="15"/>
       <c r="K37" s="15"/>
@@ -994,20 +1310,11 @@
       <c r="P37" s="15"/>
       <c r="Q37" s="15"/>
       <c r="R37" s="15"/>
-      <c r="T37"/>
-      <c r="U37"/>
-      <c r="V37"/>
-      <c r="W37"/>
-      <c r="X37"/>
-      <c r="Y37"/>
-    </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B39" s="15"/>
-      <c r="C39"/>
-      <c r="D39"/>
       <c r="F39" s="16"/>
       <c r="G39" s="16"/>
-      <c r="H39"/>
       <c r="I39" s="16"/>
       <c r="J39" s="15"/>
       <c r="K39" s="15"/>
@@ -1018,12 +1325,6 @@
       <c r="P39" s="15"/>
       <c r="Q39" s="15"/>
       <c r="R39" s="15"/>
-      <c r="T39"/>
-      <c r="U39"/>
-      <c r="V39"/>
-      <c r="W39"/>
-      <c r="X39"/>
-      <c r="Y39"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1048,108 +1349,108 @@
   <sheetData>
     <row r="1" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
       <c r="B4" s="10" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11"/>
       <c r="B5" s="10" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11"/>
       <c r="B6" s="10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C6" s="9"/>
     </row>
     <row r="7" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="11"/>
       <c r="B7" s="10" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C7" s="9"/>
     </row>
     <row r="8" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11"/>
       <c r="B8" s="10" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C8" s="9"/>
     </row>
     <row r="9" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11"/>
       <c r="B9" s="10" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C9" s="9"/>
     </row>
     <row r="10" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11"/>
       <c r="B10" s="10" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C10" s="9"/>
     </row>
     <row r="11" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="11"/>
       <c r="B11" s="10" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C11" s="9"/>
     </row>
     <row r="12" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11"/>
       <c r="B12" s="10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C12" s="9"/>
     </row>
     <row r="13" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="11"/>
       <c r="B13" s="10" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C13" s="9"/>
     </row>

</xml_diff>

<commit_message>
Added support for overriding defaul 50m slope length. Updated libraries for aiohttp and urllib3.
</commit_message>
<xml_diff>
--- a/RHEM_template.xlsx
+++ b/RHEM_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gerardo/my/Projects/RHEM/RHEM_batch_app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3F8A690-922A-F246-A208-4072923D4BCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4D43878-4E1A-864E-87A3-D834F77705A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="51200" windowHeight="28280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -639,7 +639,7 @@
   <dimension ref="A1:AA39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X14" sqref="X14"/>
+      <selection activeCell="T2" sqref="T2:X5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -810,11 +810,8 @@
     <row r="3" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A3" s="14"/>
       <c r="B3" s="15"/>
-      <c r="C3"/>
-      <c r="D3"/>
       <c r="F3" s="16"/>
       <c r="G3" s="16"/>
-      <c r="H3"/>
       <c r="I3" s="16"/>
       <c r="J3" s="15"/>
       <c r="K3" s="15"/>
@@ -825,20 +822,12 @@
       <c r="P3" s="15"/>
       <c r="Q3" s="15"/>
       <c r="R3" s="15"/>
-      <c r="T3"/>
-      <c r="U3"/>
-      <c r="V3"/>
-      <c r="W3"/>
-      <c r="X3"/>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A4" s="14"/>
       <c r="B4" s="15"/>
-      <c r="C4"/>
-      <c r="D4"/>
       <c r="F4" s="16"/>
       <c r="G4" s="16"/>
-      <c r="H4"/>
       <c r="I4" s="16"/>
       <c r="J4" s="15"/>
       <c r="K4" s="15"/>
@@ -849,20 +838,12 @@
       <c r="P4" s="15"/>
       <c r="Q4" s="15"/>
       <c r="R4" s="15"/>
-      <c r="T4"/>
-      <c r="U4"/>
-      <c r="V4"/>
-      <c r="W4"/>
-      <c r="X4"/>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A5" s="14"/>
       <c r="B5" s="15"/>
-      <c r="C5"/>
-      <c r="D5"/>
       <c r="F5" s="16"/>
       <c r="G5" s="16"/>
-      <c r="H5"/>
       <c r="I5" s="16"/>
       <c r="J5" s="15"/>
       <c r="K5" s="15"/>
@@ -873,20 +854,12 @@
       <c r="P5" s="15"/>
       <c r="Q5" s="15"/>
       <c r="R5" s="15"/>
-      <c r="T5"/>
-      <c r="U5"/>
-      <c r="V5"/>
-      <c r="W5"/>
-      <c r="X5"/>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A6" s="14"/>
       <c r="B6" s="15"/>
-      <c r="C6"/>
-      <c r="D6"/>
       <c r="F6" s="16"/>
       <c r="G6" s="16"/>
-      <c r="H6"/>
       <c r="I6" s="16"/>
       <c r="J6" s="15"/>
       <c r="K6" s="15"/>
@@ -897,20 +870,12 @@
       <c r="P6" s="15"/>
       <c r="Q6" s="15"/>
       <c r="R6" s="15"/>
-      <c r="T6"/>
-      <c r="U6"/>
-      <c r="V6"/>
-      <c r="W6"/>
-      <c r="X6"/>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A7" s="14"/>
       <c r="B7" s="15"/>
-      <c r="C7"/>
-      <c r="D7"/>
       <c r="F7" s="16"/>
       <c r="G7" s="16"/>
-      <c r="H7"/>
       <c r="I7" s="16"/>
       <c r="J7" s="15"/>
       <c r="K7" s="15"/>
@@ -921,20 +886,12 @@
       <c r="P7" s="15"/>
       <c r="Q7" s="15"/>
       <c r="R7" s="15"/>
-      <c r="T7"/>
-      <c r="U7"/>
-      <c r="V7"/>
-      <c r="W7"/>
-      <c r="X7"/>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A8" s="14"/>
       <c r="B8" s="15"/>
-      <c r="C8"/>
-      <c r="D8"/>
       <c r="F8" s="16"/>
       <c r="G8" s="16"/>
-      <c r="H8"/>
       <c r="I8" s="16"/>
       <c r="J8" s="15"/>
       <c r="K8" s="15"/>
@@ -945,20 +902,12 @@
       <c r="P8" s="15"/>
       <c r="Q8" s="15"/>
       <c r="R8" s="15"/>
-      <c r="T8"/>
-      <c r="U8"/>
-      <c r="V8"/>
-      <c r="W8"/>
-      <c r="X8"/>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A9" s="14"/>
       <c r="B9" s="15"/>
-      <c r="C9"/>
-      <c r="D9"/>
       <c r="F9" s="16"/>
       <c r="G9" s="16"/>
-      <c r="H9"/>
       <c r="I9" s="16"/>
       <c r="J9" s="15"/>
       <c r="K9" s="15"/>
@@ -969,20 +918,12 @@
       <c r="P9" s="15"/>
       <c r="Q9" s="15"/>
       <c r="R9" s="15"/>
-      <c r="T9"/>
-      <c r="U9"/>
-      <c r="V9"/>
-      <c r="W9"/>
-      <c r="X9"/>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A10" s="14"/>
       <c r="B10" s="15"/>
-      <c r="C10"/>
-      <c r="D10"/>
       <c r="F10" s="16"/>
       <c r="G10" s="16"/>
-      <c r="H10"/>
       <c r="I10" s="16"/>
       <c r="J10" s="15"/>
       <c r="K10" s="15"/>
@@ -993,20 +934,12 @@
       <c r="P10" s="15"/>
       <c r="Q10" s="15"/>
       <c r="R10" s="15"/>
-      <c r="T10"/>
-      <c r="U10"/>
-      <c r="V10"/>
-      <c r="W10"/>
-      <c r="X10"/>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A11" s="14"/>
       <c r="B11" s="15"/>
-      <c r="C11"/>
-      <c r="D11"/>
       <c r="F11" s="16"/>
       <c r="G11" s="16"/>
-      <c r="H11"/>
       <c r="I11" s="16"/>
       <c r="J11" s="15"/>
       <c r="K11" s="15"/>
@@ -1017,20 +950,12 @@
       <c r="P11" s="15"/>
       <c r="Q11" s="15"/>
       <c r="R11" s="15"/>
-      <c r="T11"/>
-      <c r="U11"/>
-      <c r="V11"/>
-      <c r="W11"/>
-      <c r="X11"/>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A12" s="14"/>
       <c r="B12" s="15"/>
-      <c r="C12"/>
-      <c r="D12"/>
       <c r="F12" s="16"/>
       <c r="G12" s="16"/>
-      <c r="H12"/>
       <c r="I12" s="16"/>
       <c r="J12" s="15"/>
       <c r="K12" s="15"/>
@@ -1041,20 +966,12 @@
       <c r="P12" s="15"/>
       <c r="Q12" s="15"/>
       <c r="R12" s="15"/>
-      <c r="T12"/>
-      <c r="U12"/>
-      <c r="V12"/>
-      <c r="W12"/>
-      <c r="X12"/>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A13" s="14"/>
       <c r="B13" s="15"/>
-      <c r="C13"/>
-      <c r="D13"/>
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
-      <c r="H13"/>
       <c r="I13" s="16"/>
       <c r="J13" s="15"/>
       <c r="K13" s="15"/>
@@ -1065,20 +982,12 @@
       <c r="P13" s="15"/>
       <c r="Q13" s="15"/>
       <c r="R13" s="15"/>
-      <c r="T13"/>
-      <c r="U13"/>
-      <c r="V13"/>
-      <c r="W13"/>
-      <c r="X13"/>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A14" s="14"/>
       <c r="B14" s="15"/>
-      <c r="C14"/>
-      <c r="D14"/>
       <c r="F14" s="16"/>
       <c r="G14" s="16"/>
-      <c r="H14"/>
       <c r="I14" s="16"/>
       <c r="J14" s="15"/>
       <c r="K14" s="15"/>
@@ -1089,20 +998,12 @@
       <c r="P14" s="15"/>
       <c r="Q14" s="15"/>
       <c r="R14" s="15"/>
-      <c r="T14"/>
-      <c r="U14"/>
-      <c r="V14"/>
-      <c r="W14"/>
-      <c r="X14"/>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A15" s="14"/>
       <c r="B15" s="15"/>
-      <c r="C15"/>
-      <c r="D15"/>
       <c r="F15" s="16"/>
       <c r="G15" s="16"/>
-      <c r="H15"/>
       <c r="I15" s="16"/>
       <c r="J15" s="15"/>
       <c r="K15" s="15"/>
@@ -1113,20 +1014,12 @@
       <c r="P15" s="15"/>
       <c r="Q15" s="15"/>
       <c r="R15" s="15"/>
-      <c r="T15"/>
-      <c r="U15"/>
-      <c r="V15"/>
-      <c r="W15"/>
-      <c r="X15"/>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A16" s="14"/>
       <c r="B16" s="15"/>
-      <c r="C16"/>
-      <c r="D16"/>
       <c r="F16" s="16"/>
       <c r="G16" s="16"/>
-      <c r="H16"/>
       <c r="I16" s="16"/>
       <c r="J16" s="15"/>
       <c r="K16" s="15"/>
@@ -1137,20 +1030,12 @@
       <c r="P16" s="15"/>
       <c r="Q16" s="15"/>
       <c r="R16" s="15"/>
-      <c r="T16"/>
-      <c r="U16"/>
-      <c r="V16"/>
-      <c r="W16"/>
-      <c r="X16"/>
-    </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" s="14"/>
       <c r="B17" s="15"/>
-      <c r="C17"/>
-      <c r="D17"/>
       <c r="F17" s="16"/>
       <c r="G17" s="16"/>
-      <c r="H17"/>
       <c r="I17" s="16"/>
       <c r="J17" s="15"/>
       <c r="K17" s="15"/>
@@ -1161,20 +1046,12 @@
       <c r="P17" s="15"/>
       <c r="Q17" s="15"/>
       <c r="R17" s="15"/>
-      <c r="T17"/>
-      <c r="U17"/>
-      <c r="V17"/>
-      <c r="W17"/>
-      <c r="X17"/>
-    </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" s="14"/>
       <c r="B18" s="15"/>
-      <c r="C18"/>
-      <c r="D18"/>
       <c r="F18" s="16"/>
       <c r="G18" s="16"/>
-      <c r="H18"/>
       <c r="I18" s="16"/>
       <c r="J18" s="15"/>
       <c r="K18" s="15"/>
@@ -1185,20 +1062,12 @@
       <c r="P18" s="15"/>
       <c r="Q18" s="15"/>
       <c r="R18" s="15"/>
-      <c r="T18"/>
-      <c r="U18"/>
-      <c r="V18"/>
-      <c r="W18"/>
-      <c r="X18"/>
-    </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" s="14"/>
       <c r="B19" s="15"/>
-      <c r="C19"/>
-      <c r="D19"/>
       <c r="F19" s="16"/>
       <c r="G19" s="16"/>
-      <c r="H19"/>
       <c r="I19" s="16"/>
       <c r="J19" s="15"/>
       <c r="K19" s="15"/>
@@ -1209,20 +1078,12 @@
       <c r="P19" s="15"/>
       <c r="Q19" s="15"/>
       <c r="R19" s="15"/>
-      <c r="T19"/>
-      <c r="U19"/>
-      <c r="V19"/>
-      <c r="W19"/>
-      <c r="X19"/>
-    </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20" s="14"/>
       <c r="B20" s="15"/>
-      <c r="C20"/>
-      <c r="D20"/>
       <c r="F20" s="16"/>
       <c r="G20" s="16"/>
-      <c r="H20"/>
       <c r="I20" s="16"/>
       <c r="J20" s="15"/>
       <c r="K20" s="15"/>
@@ -1233,20 +1094,12 @@
       <c r="P20" s="15"/>
       <c r="Q20" s="15"/>
       <c r="R20" s="15"/>
-      <c r="T20"/>
-      <c r="U20"/>
-      <c r="V20"/>
-      <c r="W20"/>
-      <c r="X20"/>
-    </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" s="14"/>
       <c r="B21" s="15"/>
-      <c r="C21"/>
-      <c r="D21"/>
       <c r="F21" s="16"/>
       <c r="G21" s="16"/>
-      <c r="H21"/>
       <c r="I21" s="16"/>
       <c r="J21" s="15"/>
       <c r="K21" s="15"/>
@@ -1257,11 +1110,6 @@
       <c r="P21" s="15"/>
       <c r="Q21" s="15"/>
       <c r="R21" s="15"/>
-      <c r="T21"/>
-      <c r="U21"/>
-      <c r="V21"/>
-      <c r="W21"/>
-      <c r="X21"/>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A33" s="14"/>

</xml_diff>